<commit_message>
generación de los archivos de la evidencia2
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/ingestion.xlsx
+++ b/src/bigdata/static/xlsx/ingestion.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,17 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>plataformas</t>
+          <t>desarrolladores</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>año</t>
+          <t>publicadores</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fechas_lanzamiento</t>
         </is>
       </c>
     </row>
@@ -476,12 +481,17 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Lucid Sheep Games</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Lucid Sheep Games</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "April 12, 2018", "Europe": "April 12, 2018", "Australia": "April 12, 2018"}</t>
         </is>
       </c>
     </row>
@@ -501,12 +511,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Beatshapers</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Beatshapers</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "January 24, 2019", "Europe": "January 24, 2019", "Australia": "January 24, 2019"}</t>
         </is>
       </c>
     </row>
@@ -526,12 +541,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>QubicGames</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>QubicGames</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "August 9, 2019", "Europe": "August 9, 2019", "Australia": "August 9, 2019"}</t>
         </is>
       </c>
     </row>
@@ -551,12 +571,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Skobbejak Games</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Skobbejak Games</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "November 6, 2018", "Europe": "December 7, 2018", "Australia": "December 7, 2018"}</t>
         </is>
       </c>
     </row>
@@ -576,12 +601,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Nintendo EPD</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Nintendo</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>{"Japan": "March 3, 2017", "NorthAmerica": "March 3, 2017", "Europe": "March 3, 2017", "Australia": "March 3, 2017"}</t>
         </is>
       </c>
     </row>
@@ -601,12 +631,17 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Blue Print</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Blue Print</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>{"Japan": "December 21, 2017", "NorthAmerica": "January 25, 2018", "Europe": "February 22, 2018", "Australia": "February 22, 2018"}</t>
         </is>
       </c>
     </row>
@@ -626,12 +661,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Nawia Games</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Nawia Games</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "October 25, 2018", "Europe": "October 25, 2018", "Australia": "October 25, 2018"}</t>
         </is>
       </c>
     </row>
@@ -651,12 +691,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Ink Stains Games</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>HypeTrain Digital</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "March 5, 2019", "Europe": "March 5, 2019", "Australia": "March 5, 2019"}</t>
         </is>
       </c>
     </row>
@@ -676,12 +721,17 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Jetdogs, Zoom Out Games</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>JetDogs</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "March 24, 2019", "Europe": "April 1, 2019", "Australia": "April 1, 2019"}</t>
         </is>
       </c>
     </row>
@@ -701,12 +751,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Roman Uhilg</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Roman Uhilg</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>{"Japan": "April 26, 2018", "NorthAmerica": "April 27, 2018", "Europe": "April 27, 2018", "Australia": "April 27, 2018"}</t>
         </is>
       </c>
     </row>
@@ -726,12 +781,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Carlsen Games</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Carlsen Games</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "January 9, 2019", "Europe": "January 9, 2019", "Australia": "January 9, 2019"}</t>
         </is>
       </c>
     </row>
@@ -751,12 +811,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Andrade Games</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Korion</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "June 14, 2018", "Europe": "June 14, 2018", "Australia": "June 14, 2018"}</t>
         </is>
       </c>
     </row>
@@ -776,12 +841,17 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Ink Stories</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Ink Stories</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "August 2, 2018", "Europe": "August 2, 2018", "Australia": "August 2, 2018"}</t>
         </is>
       </c>
     </row>
@@ -801,12 +871,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Baltoro Games</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Baltoro Games</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "September 20, 2019", "Europe": "September 20, 2019", "Australia": "September 20, 2019"}</t>
         </is>
       </c>
     </row>
@@ -826,12 +901,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Millo Games</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Millo Games</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "December 23, 2019", "Europe": "December 23, 2019", "Australia": "December 23, 2019"}</t>
         </is>
       </c>
     </row>
@@ -851,12 +931,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>MidBoss</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>MidBoss</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>{"Japan": "December 27, 2018", "NorthAmerica": "August 14, 2018", "Europe": "August 14, 2018", "Australia": "August 14, 2018"}</t>
         </is>
       </c>
     </row>
@@ -876,12 +961,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Batterystaple Games</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Batterystaple Games</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>{"Japan": "July 10, 2018", "NorthAmerica": "July 10, 2018", "Europe": "July 10, 2018", "Australia": "July 10, 2018"}</t>
         </is>
       </c>
     </row>
@@ -901,12 +991,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Digital Bards</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Digital Bards</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>{"Japan": "February 21, 2019", "NorthAmerica": "May 30, 2019", "Europe": "May 30, 2019", "Australia": "May 30, 2019"}</t>
         </is>
       </c>
     </row>
@@ -926,12 +1021,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Petite Games</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>JP: Rainy Frog, WW: Ratalaika Games</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>{"Japan": "September 27, 2017", "NorthAmerica": "September 14, 2017", "Europe": "September 14, 2017", "Australia": "September 14, 2017"}</t>
         </is>
       </c>
     </row>
@@ -951,12 +1051,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Joindots</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Desconocido</t>
+          <t>Joindots</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>{"Japan": "Unreleased", "NorthAmerica": "February 1, 2018", "Europe": "February 1, 2018", "Australia": "February 1, 2018"}</t>
         </is>
       </c>
     </row>

</xml_diff>